<commit_message>
fix xuat tkb lop va truong
</commit_message>
<xml_diff>
--- a/public/export/thoikhoabieutruong.xlsx
+++ b/public/export/thoikhoabieutruong.xlsx
@@ -1824,24 +1824,12 @@
       <c r="B13" s="6">
         <v>2</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
@@ -1885,24 +1873,12 @@
       <c r="B14" s="6">
         <v>3</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
@@ -1946,24 +1922,12 @@
       <c r="B15" s="6">
         <v>4</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -2007,24 +1971,12 @@
       <c r="B16" s="6">
         <v>5</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>

</xml_diff>